<commit_message>
all steps complete, including export
</commit_message>
<xml_diff>
--- a/code/SubjectsTable.xlsx
+++ b/code/SubjectsTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Niko\Corenats2020\CORENATS2020\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbusch\DOCUME~1\MobaXterm\slash\RemoteFiles\198582_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB03ED7-46A8-4F7C-BDBB-AD432F95A872}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847CB7D2-BB88-4529-8DB9-801545AC0E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,7 +273,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -591,7 +591,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="2" customWidth="1"/>
@@ -993,7 +993,7 @@
         <v>32</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>33</v>

</xml_diff>